<commit_message>
Update demo dataset with more articles
</commit_message>
<xml_diff>
--- a/data/articles_demo.xlsx
+++ b/data/articles_demo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,12 +458,63 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Article de test</t>
+          <t>Article sur l économie</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Ceci est un article de test pour démontrer le fonctionnement du chatbot.</t>
+          <t>L économie mondiale montre des signes de reprise...</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-01-15</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Actualités politiques</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Les dernières décisions politiques impactent...</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-02-01</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Innovations technologiques</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Les nouvelles technologies révolutionnent...</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-02-15</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Développement durable</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Les initiatives environnementales progressent...</t>
         </is>
       </c>
     </row>

</xml_diff>